<commit_message>
Improve query handling; Add synonym mapping & fuzzy matching
</commit_message>
<xml_diff>
--- a/ai_robotics_qa.xlsx
+++ b/ai_robotics_qa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Desktop\internship\robotics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Whale/for MAC/Enlight Wisdom Internship 2025/snowman/StreamlitChatbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A639A6CE-7F02-45B0-B25C-80EE123E607E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8112F3F9-0E70-B446-93A2-2074BC37C3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="i need an excel file with 50 ba" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Question</t>
   </si>
@@ -326,13 +326,19 @@
   </si>
   <si>
     <t>Fuzzy logic is a form of many-valued logic in which the truth values of variables may be any real number between 0 and 1, inclusive.</t>
+  </si>
+  <si>
+    <t>What are sensors?</t>
+  </si>
+  <si>
+    <t>A sensor is a device that detects changes in its environment and responds by generating a signal that can be measured and used for various purposes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -350,6 +356,13 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -372,10 +385,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,13 +610,18 @@
   </sheetPr>
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="40.1640625" customWidth="1"/>
+    <col min="2" max="2" width="118.5" customWidth="1"/>
+    <col min="9" max="9" width="29.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -618,7 +637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -626,7 +645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -634,7 +653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -642,7 +661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -650,7 +669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -658,7 +677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -666,7 +685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -674,7 +693,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -682,7 +701,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -690,7 +709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -698,7 +717,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -706,7 +725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -714,7 +733,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -722,7 +741,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -730,7 +749,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -738,7 +757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -746,7 +765,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -754,7 +773,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -762,7 +781,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -770,7 +789,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -778,7 +797,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -786,7 +805,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -794,7 +813,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -802,7 +821,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -810,7 +829,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -818,7 +837,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -826,7 +845,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -834,7 +853,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -842,7 +861,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
@@ -850,7 +869,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -858,7 +877,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -866,7 +885,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
@@ -874,7 +893,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -882,7 +901,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
@@ -890,7 +909,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
@@ -898,7 +917,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
@@ -906,7 +925,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
@@ -914,7 +933,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
@@ -922,7 +941,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
@@ -930,7 +949,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -938,7 +957,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -946,7 +965,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
@@ -954,7 +973,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
@@ -962,7 +981,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
@@ -970,7 +989,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
@@ -978,7 +997,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -986,7 +1005,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
@@ -994,7 +1013,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -1002,7 +1021,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
@@ -1010,52 +1029,57 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="2"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="2"/>
     </row>
   </sheetData>

</xml_diff>